<commit_message>
To Do List Excel Template
</commit_message>
<xml_diff>
--- a/To-Do_List_Template.xlsx
+++ b/To-Do_List_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sriram/projects/github/util/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sriram/projects/gh/playground/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -82,16 +82,7 @@
     <t>To-Do List!</t>
   </si>
   <si>
-    <t>Task due today</t>
-  </si>
-  <si>
     <t>Task past due!</t>
-  </si>
-  <si>
-    <t>Task due in the future</t>
-  </si>
-  <si>
-    <t>Completed task</t>
   </si>
   <si>
     <t>Category 4</t>
@@ -107,6 +98,15 @@
   </si>
   <si>
     <t>4. Low</t>
+  </si>
+  <si>
+    <t>Task due in the future!</t>
+  </si>
+  <si>
+    <t>Completed task!</t>
+  </si>
+  <si>
+    <t>Task due today!</t>
   </si>
 </sst>
 </file>
@@ -8766,7 +8766,7 @@
   <dimension ref="B1:G1004"/>
   <sheetViews>
     <sheetView showGridLines="0" showRuler="0" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:G5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8822,7 +8822,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="E6" s="9">
         <f ca="1">B3</f>
@@ -8839,7 +8839,7 @@
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="9">
         <f ca="1">E6-5</f>
@@ -8856,7 +8856,7 @@
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E8" s="9">
         <f ca="1">E6+5</f>
@@ -8869,13 +8869,13 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E9" s="9">
         <f ca="1">E6-1</f>
@@ -16914,7 +16914,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -16935,22 +16935,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>